<commit_message>
update DCCD + 3 mm
</commit_message>
<xml_diff>
--- a/data/orientations/narrowwidescan_2021-07-07_v2.xlsx
+++ b/data/orientations/narrowwidescan_2021-07-07_v2.xlsx
@@ -456,10 +456,10 @@
         <v>-1353.67060238155</v>
       </c>
       <c r="H2">
-        <v>149.1583866451164</v>
+        <v>151.5656107402997</v>
       </c>
       <c r="I2">
-        <v>0.1090345306223285</v>
+        <v>0.147687521460849</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
@@ -488,10 +488,10 @@
         <v>-1227.379635126169</v>
       </c>
       <c r="H3">
-        <v>149.6021228343545</v>
+        <v>152.005938202548</v>
       </c>
       <c r="I3">
-        <v>0.08002057777145213</v>
+        <v>0.108366465094989</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
@@ -520,10 +520,10 @@
         <v>-132.5805593341865</v>
       </c>
       <c r="H4">
-        <v>149.5617461134991</v>
+        <v>151.9683761157657</v>
       </c>
       <c r="I4">
-        <v>0.06881423284799582</v>
+        <v>0.09319680967445086</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
@@ -552,10 +552,10 @@
         <v>-132.6900054304294</v>
       </c>
       <c r="H5">
-        <v>149.6006217221812</v>
+        <v>152.0126328074481</v>
       </c>
       <c r="I5">
-        <v>0.0799978989807774</v>
+        <v>0.1083533325169687</v>
       </c>
       <c r="J5" t="b">
         <v>0</v>
@@ -584,10 +584,10 @@
         <v>-143.9759225384453</v>
       </c>
       <c r="H6">
-        <v>149.6004216645964</v>
+        <v>152.0115151722061</v>
       </c>
       <c r="I6">
-        <v>0.08573241935334135</v>
+        <v>0.1161183228880781</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
@@ -616,10 +616,10 @@
         <v>-1822.881609282897</v>
       </c>
       <c r="H7">
-        <v>151.5846789371751</v>
+        <v>154.0391088967869</v>
       </c>
       <c r="I7">
-        <v>0.1664707799182016</v>
+        <v>0.2255241205133006</v>
       </c>
       <c r="J7" t="b">
         <v>0</v>
@@ -648,10 +648,10 @@
         <v>-1222.097148368361</v>
       </c>
       <c r="H8">
-        <v>151.5994916732805</v>
+        <v>154.0524486596971</v>
       </c>
       <c r="I8">
-        <v>0.133581298382327</v>
+        <v>0.1809617531730773</v>
       </c>
       <c r="J8" t="b">
         <v>0</v>
@@ -680,10 +680,10 @@
         <v>-619.0285889318895</v>
       </c>
       <c r="H9">
-        <v>152.7928264179756</v>
+        <v>155.2666129994101</v>
       </c>
       <c r="I9">
-        <v>0.1565262132060353</v>
+        <v>0.2120535616338871</v>
       </c>
       <c r="J9" t="b">
         <v>0</v>
@@ -712,10 +712,10 @@
         <v>-12.27685326021196</v>
       </c>
       <c r="H10">
-        <v>153.4048929919806</v>
+        <v>155.888396467415</v>
       </c>
       <c r="I10">
-        <v>0.1646012759784031</v>
+        <v>0.2229883299108782</v>
       </c>
       <c r="J10" t="b">
         <v>0</v>
@@ -744,10 +744,10 @@
         <v>594.073070296512</v>
       </c>
       <c r="H11">
-        <v>149.3564547377518</v>
+        <v>151.7750850039336</v>
       </c>
       <c r="I11">
-        <v>0.121741927109218</v>
+        <v>0.1649269456388452</v>
       </c>
       <c r="J11" t="b">
         <v>0</v>
@@ -776,10 +776,10 @@
         <v>1201.233228772914</v>
       </c>
       <c r="H12">
-        <v>148.4137262534354</v>
+        <v>150.8166232066449</v>
       </c>
       <c r="I12">
-        <v>0.1295900227547318</v>
+        <v>0.1755595128831169</v>
       </c>
       <c r="J12" t="b">
         <v>0</v>
@@ -808,10 +808,10 @@
         <v>-1333.437055135223</v>
       </c>
       <c r="H13">
-        <v>148.9411078854495</v>
+        <v>151.3417261093441</v>
       </c>
       <c r="I13">
-        <v>0.09247350814636772</v>
+        <v>0.1252485475220408</v>
       </c>
       <c r="J13" t="b">
         <v>0</v>
@@ -840,10 +840,10 @@
         <v>-726.962841151636</v>
       </c>
       <c r="H14">
-        <v>148.9691767884996</v>
+        <v>151.3656736527939</v>
       </c>
       <c r="I14">
-        <v>0.08901664197770846</v>
+        <v>0.1205553893788476</v>
       </c>
       <c r="J14" t="b">
         <v>0</v>
@@ -872,10 +872,10 @@
         <v>-119.2528443922629</v>
       </c>
       <c r="H15">
-        <v>149.763693404869</v>
+        <v>152.1741395845495</v>
       </c>
       <c r="I15">
-        <v>0.0966810401888329</v>
+        <v>0.1309390400281521</v>
       </c>
       <c r="J15" t="b">
         <v>0</v>
@@ -904,10 +904,10 @@
         <v>1093.529424563656</v>
       </c>
       <c r="H16">
-        <v>153.2609610648922</v>
+        <v>155.7401109774144</v>
       </c>
       <c r="I16">
-        <v>0.1393949859964001</v>
+        <v>0.1888335954364468</v>
       </c>
       <c r="J16" t="b">
         <v>0</v>
@@ -936,10 +936,10 @@
         <v>-1440.511502610707</v>
       </c>
       <c r="H17">
-        <v>149.6562541974774</v>
+        <v>152.0699525618234</v>
       </c>
       <c r="I17">
-        <v>0.07646793402530296</v>
+        <v>0.1035737638768537</v>
       </c>
       <c r="J17" t="b">
         <v>0</v>
@@ -968,10 +968,10 @@
         <v>-833.6374728422688</v>
       </c>
       <c r="H18">
-        <v>149.6831923703429</v>
+        <v>152.0937504175068</v>
       </c>
       <c r="I18">
-        <v>0.09084646762043565</v>
+        <v>0.1230403917271251</v>
       </c>
       <c r="J18" t="b">
         <v>0</v>
@@ -1000,10 +1000,10 @@
         <v>-228.2971259854348</v>
       </c>
       <c r="H19">
-        <v>149.8746483279422</v>
+        <v>152.2840680321257</v>
       </c>
       <c r="I19">
-        <v>0.07028972297585984</v>
+        <v>0.09519074387375316</v>
       </c>
       <c r="J19" t="b">
         <v>0</v>
@@ -1032,10 +1032,10 @@
         <v>986.5094024181581</v>
       </c>
       <c r="H20">
-        <v>149.623239869722</v>
+        <v>152.0328472766903</v>
       </c>
       <c r="I20">
-        <v>0.09098549563784017</v>
+        <v>0.1232287693425566</v>
       </c>
       <c r="J20" t="b">
         <v>0</v>
@@ -1064,10 +1064,10 @@
         <v>-1543.681261375496</v>
       </c>
       <c r="H21">
-        <v>155.2994830653004</v>
+        <v>157.7916612115569</v>
       </c>
       <c r="I21">
-        <v>0.08082945400871042</v>
+        <v>0.1094551823307176</v>
       </c>
       <c r="J21" t="b">
         <v>0</v>
@@ -1096,10 +1096,10 @@
         <v>-938.0841566617896</v>
       </c>
       <c r="H22">
-        <v>149.5296740441645</v>
+        <v>151.9414710742979</v>
       </c>
       <c r="I22">
-        <v>0.07718199435407191</v>
+        <v>0.104541251533543</v>
       </c>
       <c r="J22" t="b">
         <v>0</v>
@@ -1128,10 +1128,10 @@
         <v>-329.8009440793221</v>
       </c>
       <c r="H23">
-        <v>149.681961660399</v>
+        <v>152.0897904988037</v>
       </c>
       <c r="I23">
-        <v>0.0757549089611482</v>
+        <v>0.1025951813059523</v>
       </c>
       <c r="J23" t="b">
         <v>0</v>
@@ -1160,10 +1160,10 @@
         <v>279.2227247012138</v>
       </c>
       <c r="H24">
-        <v>150.0449424935597</v>
+        <v>152.4628663311817</v>
       </c>
       <c r="I24">
-        <v>0.08396378421812986</v>
+        <v>0.1137220878179702</v>
       </c>
       <c r="J24" t="b">
         <v>0</v>
@@ -1192,10 +1192,10 @@
         <v>888.8498826465461</v>
       </c>
       <c r="H25">
-        <v>149.7458990106424</v>
+        <v>152.154778507928</v>
       </c>
       <c r="I25">
-        <v>0.07557221911451907</v>
+        <v>0.1023477671918774</v>
       </c>
       <c r="J25" t="b">
         <v>0</v>
@@ -1256,10 +1256,10 @@
         <v>164.9185457315102</v>
       </c>
       <c r="H27">
-        <v>149.5734609702966</v>
+        <v>151.9819786895464</v>
       </c>
       <c r="I27">
-        <v>0.08949897540849279</v>
+        <v>0.1212146117422016</v>
       </c>
       <c r="J27" t="b">
         <v>0</v>
@@ -1288,10 +1288,10 @@
         <v>232.4399419986362</v>
       </c>
       <c r="H28">
-        <v>149.6341821498413</v>
+        <v>152.0467195731177</v>
       </c>
       <c r="I28">
-        <v>0.1045841299594157</v>
+        <v>0.1416509681458803</v>
       </c>
       <c r="J28" t="b">
         <v>0</v>
@@ -1320,10 +1320,10 @@
         <v>-1810.992812037694</v>
       </c>
       <c r="H29">
-        <v>149.4605618671407</v>
+        <v>151.8715862216874</v>
       </c>
       <c r="I29">
-        <v>0.0779012307848231</v>
+        <v>0.105514303983595</v>
       </c>
       <c r="J29" t="b">
         <v>0</v>
@@ -1352,10 +1352,10 @@
         <v>-1719.628021603447</v>
       </c>
       <c r="H30">
-        <v>149.5637011950031</v>
+        <v>151.9778985141396</v>
       </c>
       <c r="I30">
-        <v>0.09239785232170875</v>
+        <v>0.1251530014848004</v>
       </c>
       <c r="J30" t="b">
         <v>0</v>
@@ -1384,10 +1384,10 @@
         <v>-1625.496904328832</v>
       </c>
       <c r="H31">
-        <v>149.2459497363581</v>
+        <v>151.6539673010244</v>
       </c>
       <c r="I31">
-        <v>0.08967852103145924</v>
+        <v>0.1214680593578193</v>
       </c>
       <c r="J31" t="b">
         <v>0</v>
@@ -1416,10 +1416,10 @@
         <v>-1884.864280791075</v>
       </c>
       <c r="H32">
-        <v>148.7463729266814</v>
+        <v>151.1502515658681</v>
       </c>
       <c r="I32">
-        <v>0.0976252712448282</v>
+        <v>0.1322435614617539</v>
       </c>
       <c r="J32" t="b">
         <v>0</v>
@@ -1448,10 +1448,10 @@
         <v>-1788.423821245423</v>
       </c>
       <c r="H33">
-        <v>149.3010934487888</v>
+        <v>151.7116636126021</v>
       </c>
       <c r="I33">
-        <v>0.08178312326172854</v>
+        <v>0.1107774723696583</v>
       </c>
       <c r="J33" t="b">
         <v>0</v>
@@ -1480,10 +1480,10 @@
         <v>-1694.474333571536</v>
       </c>
       <c r="H34">
-        <v>149.0785412578464</v>
+        <v>151.4815844843498</v>
       </c>
       <c r="I34">
-        <v>0.09247247466806545</v>
+        <v>0.1252470967066953</v>
       </c>
       <c r="J34" t="b">
         <v>0</v>
@@ -1512,10 +1512,10 @@
         <v>-70.6925972440763</v>
       </c>
       <c r="H35">
-        <v>149.6353944002532</v>
+        <v>152.0470186025359</v>
       </c>
       <c r="I35">
-        <v>0.08690744745286108</v>
+        <v>0.1177096401923902</v>
       </c>
       <c r="J35" t="b">
         <v>1</v>
@@ -1544,10 +1544,10 @@
         <v>30.26592928010405</v>
       </c>
       <c r="H36">
-        <v>149.720062427067</v>
+        <v>152.1316784320978</v>
       </c>
       <c r="I36">
-        <v>0.09060810306012497</v>
+        <v>0.1227186168363573</v>
       </c>
       <c r="J36" t="b">
         <v>1</v>
@@ -1576,10 +1576,10 @@
         <v>127.1912116931339</v>
       </c>
       <c r="H37">
-        <v>149.8872405310991</v>
+        <v>152.2975699134284</v>
       </c>
       <c r="I37">
-        <v>0.07906426194105597</v>
+        <v>0.1070752069472101</v>
       </c>
       <c r="J37" t="b">
         <v>1</v>
@@ -1608,10 +1608,10 @@
         <v>227.2468452289581</v>
       </c>
       <c r="H38">
-        <v>149.6810443989948</v>
+        <v>152.0934009190962</v>
       </c>
       <c r="I38">
-        <v>0.08690676068055474</v>
+        <v>0.1177086764243578</v>
       </c>
       <c r="J38" t="b">
         <v>1</v>
@@ -1640,10 +1640,10 @@
         <v>324.5897149156522</v>
       </c>
       <c r="H39">
-        <v>150.0818342385493</v>
+        <v>152.4949482758668</v>
       </c>
       <c r="I39">
-        <v>0.1037532239743886</v>
+        <v>0.1405104642107665</v>
       </c>
       <c r="J39" t="b">
         <v>1</v>
@@ -1672,10 +1672,10 @@
         <v>425.3820512719481</v>
       </c>
       <c r="H40">
-        <v>149.8068733190853</v>
+        <v>152.2190138412069</v>
       </c>
       <c r="I40">
-        <v>0.09352533667716094</v>
+        <v>0.1266675211688783</v>
       </c>
       <c r="J40" t="b">
         <v>1</v>
@@ -1704,10 +1704,10 @@
         <v>524.1173944560242</v>
       </c>
       <c r="H41">
-        <v>150.1056226738746</v>
+        <v>152.5203401905414</v>
       </c>
       <c r="I41">
-        <v>0.1002277854727035</v>
+        <v>0.1357392528821232</v>
       </c>
       <c r="J41" t="b">
         <v>1</v>
@@ -1736,10 +1736,10 @@
         <v>-106.5228170573855</v>
       </c>
       <c r="H42">
-        <v>149.6539592759271</v>
+        <v>152.0640662767559</v>
       </c>
       <c r="I42">
-        <v>0.1024532956777081</v>
+        <v>0.1387604532006805</v>
       </c>
       <c r="J42" t="b">
         <v>1</v>
@@ -1768,10 +1768,10 @@
         <v>-7.060212000481897</v>
       </c>
       <c r="H43">
-        <v>149.6813872015272</v>
+        <v>152.08846041115</v>
       </c>
       <c r="I43">
-        <v>0.07906803517638242</v>
+        <v>0.1070804885658267</v>
       </c>
       <c r="J43" t="b">
         <v>1</v>
@@ -1800,10 +1800,10 @@
         <v>92.54051700206219</v>
       </c>
       <c r="H44">
-        <v>149.6452575703747</v>
+        <v>152.0563785797918</v>
       </c>
       <c r="I44">
-        <v>0.08886075318006413</v>
+        <v>0.1203537104700684</v>
       </c>
       <c r="J44" t="b">
         <v>1</v>
@@ -1832,10 +1832,10 @@
         <v>290.2365490777302</v>
       </c>
       <c r="H45">
-        <v>149.8652308097175</v>
+        <v>152.2735879201218</v>
       </c>
       <c r="I45">
-        <v>0.08241893872684476</v>
+        <v>0.1116148848110251</v>
       </c>
       <c r="J45" t="b">
         <v>1</v>
@@ -1864,10 +1864,10 @@
         <v>389.8473226375199</v>
       </c>
       <c r="H46">
-        <v>149.8295986116889</v>
+        <v>152.242116198506</v>
       </c>
       <c r="I46">
-        <v>0.09352522391277861</v>
+        <v>0.1266673590295916</v>
       </c>
       <c r="J46" t="b">
         <v>1</v>
@@ -1896,10 +1896,10 @@
         <v>490.5326428300518</v>
       </c>
       <c r="H47">
-        <v>149.5254570192915</v>
+        <v>151.932216149823</v>
       </c>
       <c r="I47">
-        <v>0.09357622457424172</v>
+        <v>0.1267344387142841</v>
       </c>
       <c r="J47" t="b">
         <v>1</v>
@@ -1928,10 +1928,10 @@
         <v>-141.7820730303351</v>
       </c>
       <c r="H48">
-        <v>149.9566496063346</v>
+        <v>152.3701687694523</v>
       </c>
       <c r="I48">
-        <v>0.09636525417518009</v>
+        <v>0.1305112869875901</v>
       </c>
       <c r="J48" t="b">
         <v>1</v>
@@ -1960,10 +1960,10 @@
         <v>-44.91850889484112</v>
       </c>
       <c r="H49">
-        <v>149.7615560103094</v>
+        <v>152.1737753034404</v>
       </c>
       <c r="I49">
-        <v>0.09112340400477102</v>
+        <v>0.1234163987427716</v>
       </c>
       <c r="J49" t="b">
         <v>1</v>
@@ -1992,10 +1992,10 @@
         <v>154.2423239093978</v>
       </c>
       <c r="H50">
-        <v>149.7890899303076</v>
+        <v>152.2009649183906</v>
       </c>
       <c r="I50">
-        <v>0.0935259940378958</v>
+        <v>0.1266684343392947</v>
       </c>
       <c r="J50" t="b">
         <v>1</v>
@@ -2024,10 +2024,10 @@
         <v>254.9532206578178</v>
       </c>
       <c r="H51">
-        <v>149.7132057141005</v>
+        <v>152.1200200937825</v>
       </c>
       <c r="I51">
-        <v>0.08062155940458166</v>
+        <v>0.1091827579426642</v>
       </c>
       <c r="J51" t="b">
         <v>1</v>
@@ -2056,10 +2056,10 @@
         <v>352.4265333025642</v>
       </c>
       <c r="H52">
-        <v>149.7591149602014</v>
+        <v>152.1674935914248</v>
       </c>
       <c r="I52">
-        <v>0.07862355156192313</v>
+        <v>0.1064786397919329</v>
       </c>
       <c r="J52" t="b">
         <v>1</v>
@@ -2088,10 +2088,10 @@
         <v>452.5361447057899</v>
       </c>
       <c r="H53">
-        <v>149.5157480039555</v>
+        <v>151.9270346561076</v>
       </c>
       <c r="I53">
-        <v>0.08442207247183896</v>
+        <v>0.1143448201333478</v>
       </c>
       <c r="J53" t="b">
         <v>1</v>
@@ -2120,10 +2120,10 @@
         <v>-177.1627916298978</v>
       </c>
       <c r="H54">
-        <v>149.5577620935549</v>
+        <v>151.9667388777131</v>
       </c>
       <c r="I54">
-        <v>0.09108565663847665</v>
+        <v>0.1233654465559598</v>
       </c>
       <c r="J54" t="b">
         <v>1</v>
@@ -2152,10 +2152,10 @@
         <v>-77.52836830461433</v>
       </c>
       <c r="H55">
-        <v>149.6663788998889</v>
+        <v>152.0716831063736</v>
       </c>
       <c r="I55">
-        <v>0.08195162874646174</v>
+        <v>0.1109824304626085</v>
       </c>
       <c r="J55" t="b">
         <v>1</v>
@@ -2184,10 +2184,10 @@
         <v>20.38721234550803</v>
       </c>
       <c r="H56">
-        <v>149.6514535483705</v>
+        <v>152.0572976558605</v>
       </c>
       <c r="I56">
-        <v>0.08062291028432231</v>
+        <v>0.1091846526434656</v>
       </c>
       <c r="J56" t="b">
         <v>1</v>
@@ -2216,10 +2216,10 @@
         <v>121.4755373089361</v>
       </c>
       <c r="H57">
-        <v>149.6116153204535</v>
+        <v>152.0165788028601</v>
       </c>
       <c r="I57">
-        <v>0.0861326752053104</v>
+        <v>0.1166457401855792</v>
       </c>
       <c r="J57" t="b">
         <v>1</v>
@@ -2248,10 +2248,10 @@
         <v>219.139579559454</v>
       </c>
       <c r="H58">
-        <v>149.601812153823</v>
+        <v>152.0115031615022</v>
       </c>
       <c r="I58">
-        <v>0.09108503445611341</v>
+        <v>0.1233645712220186</v>
       </c>
       <c r="J58" t="b">
         <v>1</v>
@@ -2280,10 +2280,10 @@
         <v>320.30166488958</v>
       </c>
       <c r="H59">
-        <v>149.4193889710965</v>
+        <v>151.8284493428507</v>
       </c>
       <c r="I59">
-        <v>0.0869108504944561</v>
+        <v>0.1177143689433772</v>
       </c>
       <c r="J59" t="b">
         <v>1</v>
@@ -2312,10 +2312,10 @@
         <v>417.420430013382</v>
       </c>
       <c r="H60">
-        <v>149.5399065904479</v>
+        <v>151.9510377803976</v>
       </c>
       <c r="I60">
-        <v>0.08690902861684136</v>
+        <v>0.117711815773257</v>
       </c>
       <c r="J60" t="b">
         <v>1</v>
@@ -2344,10 +2344,10 @@
         <v>-211.3222726924546</v>
       </c>
       <c r="H61">
-        <v>149.1323207384493</v>
+        <v>151.5376930428534</v>
       </c>
       <c r="I61">
-        <v>0.08981293842128661</v>
+        <v>0.1216482693420094</v>
       </c>
       <c r="J61" t="b">
         <v>1</v>
@@ -2376,10 +2376,10 @@
         <v>-112.6770518641936</v>
       </c>
       <c r="H62">
-        <v>149.6296360381595</v>
+        <v>152.0342926674716</v>
       </c>
       <c r="I62">
-        <v>0.08230340024152974</v>
+        <v>0.1114586980150636</v>
       </c>
       <c r="J62" t="b">
         <v>1</v>
@@ -2408,10 +2408,10 @@
         <v>-11.12500334239189</v>
       </c>
       <c r="H63">
-        <v>149.6291025357551</v>
+        <v>152.0355160329138</v>
       </c>
       <c r="I63">
-        <v>0.07757199864797729</v>
+        <v>0.1050548728597248</v>
       </c>
       <c r="J63" t="b">
         <v>1</v>
@@ -2440,10 +2440,10 @@
         <v>86.3774573129258</v>
       </c>
       <c r="H64">
-        <v>149.7131915402386</v>
+        <v>152.1246091290602</v>
       </c>
       <c r="I64">
-        <v>0.08940358770017738</v>
+        <v>0.121087109404861</v>
       </c>
       <c r="J64" t="b">
         <v>1</v>
@@ -2472,10 +2472,10 @@
         <v>186.8448552875502</v>
       </c>
       <c r="H65">
-        <v>149.6252703019283</v>
+        <v>152.0353634556942</v>
       </c>
       <c r="I65">
-        <v>0.08900719684869231</v>
+        <v>0.1205504444102803</v>
       </c>
       <c r="J65" t="b">
         <v>1</v>

</xml_diff>